<commit_message>
Updated Spring Backlog Tasks
</commit_message>
<xml_diff>
--- a/Sprints/Sprint1/G4CapstoneProject_Sprint1_Backlog_Burndown.xlsx
+++ b/Sprints/Sprint1/G4CapstoneProject_Sprint1_Backlog_Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Desktop\Capstone-Project\Sprints\Sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdena1\source\repos\Capstone-Project\Sprints\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B60762-FD02-4331-9871-A6044A0AF060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA32818-406F-4B9C-B601-BED0078EAAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1665" windowWidth="28800" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22920" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>Related User Story</t>
   </si>
@@ -48,12 +48,6 @@
   </si>
   <si>
     <t>Week 2</t>
-  </si>
-  <si>
-    <t>Week 3</t>
-  </si>
-  <si>
-    <t>Week 4</t>
   </si>
   <si>
     <t>Amount Remaining After…</t>
@@ -288,7 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -309,8 +303,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,23 +413,17 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$41:$G$41</c:f>
+              <c:f>Sheet1!$C$41:$E$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1180,13 +1166,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>111442</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
@@ -1480,10 +1466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1491,43 +1477,39 @@
     <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="71.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -1537,19 +1519,13 @@
       <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -1558,13 +1534,11 @@
         <v>0</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -1573,13 +1547,11 @@
         <v>0</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -1588,15 +1560,13 @@
         <v>0</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -1605,13 +1575,11 @@
         <v>0</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -1620,13 +1588,11 @@
         <v>0</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -1635,13 +1601,11 @@
         <v>0</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -1650,13 +1614,11 @@
         <v>2</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -1665,13 +1627,11 @@
         <v>2</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -1680,13 +1640,11 @@
         <v>0</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -1695,269 +1653,259 @@
         <v>0</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
       </c>
       <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
       </c>
       <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
       </c>
       <c r="D16" s="2">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
       </c>
       <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
       </c>
       <c r="D18" s="2">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
       </c>
       <c r="D19" s="2">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
       </c>
       <c r="D20" s="2">
-        <v>0</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
       </c>
       <c r="D21" s="2">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
       </c>
       <c r="D22" s="2">
-        <v>0</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
       </c>
       <c r="D23" s="2">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="B24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="10">
-        <v>2</v>
-      </c>
-      <c r="D24" s="11">
-        <v>0</v>
-      </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="10">
-        <v>2</v>
-      </c>
-      <c r="D25" s="11">
-        <v>0</v>
-      </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="10">
-        <v>2</v>
-      </c>
-      <c r="D26" s="11">
-        <v>0</v>
-      </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="10">
-        <v>2</v>
-      </c>
-      <c r="D27" s="11">
-        <v>0</v>
-      </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
@@ -1966,16 +1914,14 @@
         <v>0</v>
       </c>
       <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
@@ -1984,16 +1930,14 @@
         <v>0</v>
       </c>
       <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C30" s="1">
         <v>2</v>
@@ -2002,16 +1946,14 @@
         <v>0</v>
       </c>
       <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C31" s="1">
         <v>2</v>
@@ -2020,16 +1962,14 @@
         <v>0</v>
       </c>
       <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
@@ -2038,16 +1978,14 @@
         <v>0</v>
       </c>
       <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C33" s="1">
         <v>2</v>
@@ -2056,16 +1994,14 @@
         <v>0</v>
       </c>
       <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C34" s="1">
         <v>2</v>
@@ -2074,38 +2010,34 @@
         <v>0</v>
       </c>
       <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" t="s">
+      <c r="F34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2</v>
+      </c>
+      <c r="D35" s="2">
+        <v>2</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="1">
-        <v>2</v>
-      </c>
-      <c r="D35" s="2">
-        <v>2</v>
-      </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C36" s="1">
         <v>3</v>
@@ -2114,16 +2046,14 @@
         <v>0</v>
       </c>
       <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C37" s="1">
         <v>2</v>
@@ -2132,34 +2062,30 @@
         <v>0</v>
       </c>
       <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="1">
-        <v>2</v>
-      </c>
-      <c r="D38" s="2">
-        <v>0</v>
-      </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C39" s="1">
         <v>2</v>
@@ -2168,26 +2094,22 @@
         <v>0</v>
       </c>
       <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C41" s="3">
         <f>SUM(C4:C40)</f>
@@ -2195,28 +2117,20 @@
       </c>
       <c r="D41" s="3">
         <f>SUM(D4:D40)</f>
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="E41" s="3">
         <f>SUM(E4:E40)</f>
         <v>0</v>
       </c>
-      <c r="F41" s="3">
-        <f>SUM(F4:F40)</f>
-        <v>0</v>
-      </c>
-      <c r="G41" s="3">
-        <f>SUM(G4:G40)</f>
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="D2:G2"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>